<commit_message>
Refactor and fix more bugs
</commit_message>
<xml_diff>
--- a/meetings.xlsx
+++ b/meetings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simula67\repos\meeting-auto-attender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA14C25-1F52-440A-8830-0606D517F7DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47563914-56B5-4ECB-9B73-1999E198BC90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,23 +25,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Time(in format: dd-mm-yyyy hh:mm AM/PM)</t>
   </si>
   <si>
-    <t>https://us02web.zoom.us/j/84478123117?pwd=aWNab251S0tuKzY0UWJrYzlXR1ZBUT09</t>
-  </si>
-  <si>
-    <t>05-08-2021 14:30 PM</t>
-  </si>
-  <si>
-    <t>84478123117</t>
-  </si>
-  <si>
-    <t>901323</t>
-  </si>
-  <si>
     <t>Meeting ID (Leave blank if not applicable)</t>
   </si>
   <si>
@@ -49,6 +37,12 @@
   </si>
   <si>
     <t>Link</t>
+  </si>
+  <si>
+    <t>20-08-2021 12:00 PM</t>
+  </si>
+  <si>
+    <t>https://us02web.zoom.us/j/85071211231231231</t>
   </si>
 </sst>
 </file>
@@ -109,8 +103,8 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -395,7 +389,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -412,28 +406,23 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>2</v>
+      <c r="A2" s="6" t="s">
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
@@ -443,7 +432,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{62232864-ADBA-4479-97DC-9DCF620FB32E}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F0D539B1-A080-4AEF-8E8C-174D8F69C6BD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
* Support for JSON meetings list * requirements.txt updated to include pywin32 * Documentation improvements
</commit_message>
<xml_diff>
--- a/meetings.xlsx
+++ b/meetings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simula67\repos\meeting-auto-attender\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\4772096\PycharmProjects\meeting-auto-attender\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96ED1684-905F-4987-B632-7E468BA62A8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ACC423C-5AFA-4DBE-B319-9CCC6FF46108}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Link</t>
   </si>
@@ -42,7 +42,13 @@
     <t>22-08-2021 19:18</t>
   </si>
   <si>
-    <t>https://us05web.zoom.us/j/87177504375?pwd=djhvL2kxa2ZoQWdicWJzd1BiS0JLZzadblahblah</t>
+    <t>Example meeting from Excel</t>
+  </si>
+  <si>
+    <t>Comment (Optional)</t>
+  </si>
+  <si>
+    <t>https://us05web.zoom.us/j/87177504375?pwd=jhvL2kxa2ZoQWdicWd1BiS0JLZzadblahblah</t>
   </si>
 </sst>
 </file>
@@ -53,7 +59,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy\ h:mm"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -493,13 +499,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="50" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="85.7109375" bestFit="1" customWidth="1"/>
@@ -508,7 +514,7 @@
     <col min="5" max="5" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -521,17 +527,23 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="4"/>
       <c r="B3" s="2"/>
       <c r="C3" s="5"/>
@@ -542,6 +554,6 @@
     <hyperlink ref="B2" r:id="rId1" xr:uid="{BDB44362-111C-40F3-888F-942515EF6736}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>